<commit_message>
0710 Update --Ready For Deployment--
</commit_message>
<xml_diff>
--- a/wbs list.xlsx
+++ b/wbs list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tyler\OneDrive\문서\Ezenac\Project 01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ezenac\Project 01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E471261-90BF-49A3-B270-FC2D636743F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427655AE-4128-4F83-BEEE-25DBE7922E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6285" yWindow="4320" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="8055" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>프로젝트 이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -119,14 +119,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>토글메뉴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>슬라이드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>firebase deploy</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -180,6 +172,10 @@
   </si>
   <si>
     <t>2024-07-12 / 금요일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GSAP 프리로더, 타이틀 자동 스크롤, 스크롤 지시등(?), 토글메뉴, 스크롤진행도 바, 스크롤에 따른 페이지 등장, MBTI 스위치, 카드 페이저, 화살표, 마우스 좌표값에 따른 카드 틸트, 모바일 기능</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -187,9 +183,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="\%"/>
-  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -311,7 +304,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -657,13 +650,92 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -676,9 +748,6 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -751,22 +820,46 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -775,41 +868,50 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1094,10 +1196,10 @@
   <dimension ref="B1:W18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="1" width="2.625" customWidth="1"/>
     <col min="2" max="2" width="20.625" style="1" customWidth="1"/>
@@ -1106,483 +1208,493 @@
     <col min="9" max="52" width="5.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:23" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="16" t="s">
+    <row r="1" spans="2:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.65"/>
+    <row r="2" spans="2:23" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:23" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="18" t="s">
+    <row r="3" spans="2:23" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="19" t="s">
-        <v>37</v>
+      <c r="C3" s="18" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="4" spans="2:23" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="18" t="s">
+    <row r="4" spans="2:23" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="19" t="s">
-        <v>37</v>
+      <c r="C4" s="18" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="5" spans="2:23" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="20" t="s">
+    <row r="5" spans="2:23" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="46" t="s">
+      <c r="C5" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="46"/>
-      <c r="N5" s="47" t="s">
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="O5" s="47"/>
-      <c r="P5" s="47"/>
-      <c r="Q5" s="47"/>
-      <c r="R5" s="47"/>
-      <c r="S5" s="48" t="s">
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="T5" s="48"/>
-      <c r="U5" s="48"/>
-      <c r="V5" s="48"/>
-      <c r="W5" s="48"/>
+      <c r="T5" s="38"/>
+      <c r="U5" s="38"/>
+      <c r="V5" s="38"/>
+      <c r="W5" s="38"/>
     </row>
-    <row r="6" spans="2:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="2:23" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="38" t="s">
+    <row r="6" spans="2:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.65"/>
+    <row r="7" spans="2:23" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B7" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="D7" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38" t="s">
+      <c r="E7" s="39"/>
+      <c r="F7" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="38" t="s">
+      <c r="G7" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="40" t="s">
+      <c r="H7" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="42" t="s">
+      <c r="I7" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="43"/>
-      <c r="N7" s="44" t="s">
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="O7" s="44"/>
-      <c r="P7" s="44"/>
-      <c r="Q7" s="44"/>
-      <c r="R7" s="44"/>
-      <c r="S7" s="45" t="s">
+      <c r="O7" s="34"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="34"/>
+      <c r="R7" s="34"/>
+      <c r="S7" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="T7" s="45"/>
-      <c r="U7" s="45"/>
-      <c r="V7" s="45"/>
-      <c r="W7" s="45"/>
+      <c r="T7" s="35"/>
+      <c r="U7" s="35"/>
+      <c r="V7" s="35"/>
+      <c r="W7" s="35"/>
     </row>
-    <row r="8" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="28" t="s">
+    <row r="8" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="22" t="s">
+      <c r="J8" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="22" t="s">
+      <c r="K8" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="L8" s="22" t="s">
+      <c r="L8" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="M8" s="22" t="s">
+      <c r="M8" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="N8" s="23" t="s">
+      <c r="N8" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="O8" s="23" t="s">
+      <c r="O8" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="P8" s="23" t="s">
+      <c r="P8" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="Q8" s="23" t="s">
+      <c r="Q8" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="R8" s="23" t="s">
+      <c r="R8" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="S8" s="24" t="s">
+      <c r="S8" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="T8" s="24" t="s">
+      <c r="T8" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="U8" s="24" t="s">
+      <c r="U8" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="V8" s="24" t="s">
+      <c r="V8" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="W8" s="24" t="s">
+      <c r="W8" s="23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:23" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="25">
+    <row r="9" spans="2:23" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B9" s="24">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="36"/>
+        <v>32</v>
+      </c>
+      <c r="D9" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="43"/>
       <c r="F9" s="3">
         <v>45464</v>
       </c>
       <c r="G9" s="3">
-        <v>45469</v>
-      </c>
-      <c r="H9" s="32">
-        <v>0.1</v>
-      </c>
-      <c r="I9" s="29"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="6"/>
+        <v>45465</v>
+      </c>
+      <c r="H9" s="46">
+        <v>1</v>
+      </c>
+      <c r="I9" s="57"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="56"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="5"/>
     </row>
-    <row r="10" spans="2:23" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="26">
+    <row r="10" spans="2:23" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B10" s="25">
         <v>2</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="35"/>
-      <c r="F10" s="8">
+      <c r="C10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="42"/>
+      <c r="F10" s="7">
+        <v>45466</v>
+      </c>
+      <c r="G10" s="7">
         <v>45470</v>
       </c>
-      <c r="G10" s="8">
-        <v>45471</v>
-      </c>
-      <c r="H10" s="33">
-        <v>0.2</v>
-      </c>
-      <c r="I10" s="30"/>
+      <c r="H10" s="47">
+        <v>1</v>
+      </c>
+      <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="11"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="58"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="10"/>
     </row>
-    <row r="11" spans="2:23" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="26">
+    <row r="11" spans="2:23" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B11" s="25">
         <v>3</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="35"/>
-      <c r="F11" s="8">
+      <c r="C11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="42"/>
+      <c r="F11" s="7">
         <v>45471</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
         <v>45473</v>
       </c>
-      <c r="H11" s="33">
-        <v>0.3</v>
-      </c>
-      <c r="I11" s="30"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
-      <c r="T11" s="9"/>
-      <c r="U11" s="9"/>
-      <c r="V11" s="9"/>
-      <c r="W11" s="11"/>
+      <c r="H11" s="47">
+        <v>1</v>
+      </c>
+      <c r="I11" s="28"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="10"/>
     </row>
-    <row r="12" spans="2:23" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="26">
+    <row r="12" spans="2:23" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B12" s="25">
         <v>4</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="42"/>
+      <c r="F12" s="7">
+        <v>45472</v>
+      </c>
+      <c r="G12" s="7">
+        <v>45474</v>
+      </c>
+      <c r="H12" s="47">
+        <v>1</v>
+      </c>
+      <c r="I12" s="28"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="58"/>
+      <c r="P12" s="58"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="10"/>
+    </row>
+    <row r="13" spans="2:23" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B13" s="25">
+        <v>5</v>
+      </c>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="35"/>
-      <c r="F12" s="8">
+      <c r="E13" s="42"/>
+      <c r="F13" s="52">
         <v>45474</v>
       </c>
-      <c r="G12" s="8">
-        <v>45476</v>
-      </c>
-      <c r="H12" s="33">
-        <v>0.4</v>
-      </c>
-      <c r="I12" s="30"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="9"/>
-      <c r="W12" s="11"/>
+      <c r="G13" s="52">
+        <v>45477</v>
+      </c>
+      <c r="H13" s="47">
+        <v>1</v>
+      </c>
+      <c r="I13" s="28"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="10"/>
     </row>
-    <row r="13" spans="2:23" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="26">
-        <v>5</v>
-      </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="35"/>
-      <c r="F13" s="8">
-        <v>45474</v>
-      </c>
-      <c r="G13" s="8">
-        <v>45476</v>
-      </c>
-      <c r="H13" s="33">
-        <v>0.5</v>
-      </c>
-      <c r="I13" s="30"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9"/>
-      <c r="T13" s="9"/>
-      <c r="U13" s="9"/>
-      <c r="V13" s="9"/>
-      <c r="W13" s="11"/>
-    </row>
-    <row r="14" spans="2:23" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="26">
+    <row r="14" spans="2:23" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B14" s="25">
         <v>6</v>
       </c>
-      <c r="C14" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="35"/>
-      <c r="F14" s="8">
+      <c r="C14" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="54"/>
+      <c r="F14" s="53">
         <v>45477</v>
       </c>
-      <c r="G14" s="8">
-        <v>45478</v>
-      </c>
-      <c r="H14" s="33">
-        <v>0.6</v>
-      </c>
-      <c r="I14" s="30"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
+      <c r="G14" s="53">
+        <v>45483</v>
+      </c>
+      <c r="H14" s="50">
+        <v>1</v>
+      </c>
+      <c r="I14" s="28"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
       <c r="S14" s="9"/>
       <c r="T14" s="9"/>
       <c r="U14" s="9"/>
-      <c r="V14" s="9"/>
-      <c r="W14" s="11"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="10"/>
     </row>
-    <row r="15" spans="2:23" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="26">
+    <row r="15" spans="2:23" ht="75.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B15" s="25">
         <v>7</v>
       </c>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="35"/>
-      <c r="F15" s="8">
-        <v>45481</v>
-      </c>
-      <c r="G15" s="8">
-        <v>45482</v>
-      </c>
-      <c r="H15" s="33">
-        <v>0.7</v>
-      </c>
-      <c r="I15" s="30"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
       <c r="Q15" s="9"/>
       <c r="R15" s="9"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
       <c r="U15" s="9"/>
-      <c r="V15" s="9"/>
-      <c r="W15" s="11"/>
+      <c r="V15" s="8"/>
+      <c r="W15" s="10"/>
     </row>
-    <row r="16" spans="2:23" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="26">
+    <row r="16" spans="2:23" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B16" s="25">
         <v>8</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="42"/>
+      <c r="F16" s="3">
+        <v>45483</v>
+      </c>
+      <c r="G16" s="3">
+        <v>45484</v>
+      </c>
+      <c r="H16" s="44">
+        <v>0.9</v>
+      </c>
+      <c r="I16" s="28"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="10"/>
+    </row>
+    <row r="17" spans="2:23" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B17" s="26">
+        <v>9</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="35"/>
-      <c r="F16" s="8">
-        <v>45483</v>
-      </c>
-      <c r="G16" s="8">
-        <v>45484</v>
-      </c>
-      <c r="H16" s="33">
-        <v>0.9</v>
-      </c>
-      <c r="I16" s="30"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="9"/>
-      <c r="S16" s="9"/>
-      <c r="T16" s="9"/>
-      <c r="U16" s="10"/>
-      <c r="V16" s="10"/>
-      <c r="W16" s="11"/>
+      <c r="D17" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="41"/>
+      <c r="F17" s="12">
+        <v>45485</v>
+      </c>
+      <c r="G17" s="12">
+        <v>45485</v>
+      </c>
+      <c r="H17" s="45">
+        <v>1</v>
+      </c>
+      <c r="I17" s="29"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="13"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="13"/>
+      <c r="V17" s="13"/>
+      <c r="W17" s="14"/>
     </row>
-    <row r="17" spans="2:23" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="27">
-        <v>9</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="37"/>
-      <c r="F17" s="13">
-        <v>45485</v>
-      </c>
-      <c r="G17" s="13">
-        <v>45485</v>
-      </c>
-      <c r="H17" s="34">
-        <v>1</v>
-      </c>
-      <c r="I17" s="31"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="14"/>
-      <c r="S17" s="14"/>
-      <c r="T17" s="14"/>
-      <c r="U17" s="14"/>
-      <c r="V17" s="14"/>
-      <c r="W17" s="15"/>
-    </row>
-    <row r="18" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="25">
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:E15"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="I7:M7"/>
     <mergeCell ref="N7:R7"/>
@@ -1590,22 +1702,6 @@
     <mergeCell ref="I5:M5"/>
     <mergeCell ref="N5:R5"/>
     <mergeCell ref="S5:W5"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D13:E13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>